<commit_message>
Editados backgrounds da entrada do Castillo.
</commit_message>
<xml_diff>
--- a/Anotacoes/Mapeamento de gráficos de backgrounds.xlsx
+++ b/Anotacoes/Mapeamento de gráficos de backgrounds.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
   <si>
     <t>Versão</t>
   </si>
@@ -100,6 +100,9 @@
     <t>0x028420</t>
   </si>
   <si>
+    <t>0x523544</t>
+  </si>
+  <si>
     <t>Castillo - Cafeplaza</t>
   </si>
   <si>
@@ -167,6 +170,9 @@
   </si>
   <si>
     <t>0x02841C</t>
+  </si>
+  <si>
+    <t>0x5231E8</t>
   </si>
   <si>
     <t>0x028428</t>
@@ -203,13 +209,13 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -249,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -262,9 +268,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -581,7 +584,7 @@
     <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="5" width="9.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="41.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="41.29071428571429" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
@@ -679,7 +682,9 @@
       <c r="E6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4" t="s">
@@ -727,25 +732,29 @@
       <c r="C9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="E9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F10" s="4"/>
     </row>
@@ -754,14 +763,14 @@
         <v>7</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F11" s="4"/>
     </row>
@@ -770,12 +779,12 @@
         <v>7</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>10</v>
@@ -786,12 +795,12 @@
         <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>10</v>
@@ -799,10 +808,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -815,10 +824,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -831,10 +840,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -847,31 +856,33 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="4"/>
+      <c r="F17" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
@@ -881,16 +892,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>25</v>
@@ -901,63 +912,67 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="4"/>
+      <c r="F20" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F21" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F22" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>10</v>
@@ -965,15 +980,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Editados backgrounds do interior do Castillo.
</commit_message>
<xml_diff>
--- a/Anotacoes/Mapeamento de gráficos de backgrounds.xlsx
+++ b/Anotacoes/Mapeamento de gráficos de backgrounds.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="65">
   <si>
     <t>Versão</t>
   </si>
@@ -79,6 +79,9 @@
     <t>0x0283D8</t>
   </si>
   <si>
+    <t>0x50A0B8</t>
+  </si>
+  <si>
     <t>EletroVilla - Edifício da Jomon</t>
   </si>
   <si>
@@ -112,6 +115,9 @@
     <t>0x02842C</t>
   </si>
   <si>
+    <t>0x529428</t>
+  </si>
+  <si>
     <t>Castillo - Gifts</t>
   </si>
   <si>
@@ -121,6 +127,9 @@
     <t>0x028450</t>
   </si>
   <si>
+    <t>0x5382C4</t>
+  </si>
+  <si>
     <t>Castillo - Restaurant / Photo Studio</t>
   </si>
   <si>
@@ -160,6 +169,9 @@
     <t>0x0283DC</t>
   </si>
   <si>
+    <t>0x509D70</t>
+  </si>
+  <si>
     <t>0x0283EC</t>
   </si>
   <si>
@@ -181,10 +193,16 @@
     <t>0x028430</t>
   </si>
   <si>
+    <t>0x5290D0</t>
+  </si>
+  <si>
     <t>0x02844C</t>
   </si>
   <si>
     <t>0x028454</t>
+  </si>
+  <si>
+    <t>0x5381E8</t>
   </si>
   <si>
     <t>0x0284F4</t>
@@ -696,9 +714,11 @@
       <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="E7" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F7" s="4"/>
     </row>
@@ -707,16 +727,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>10</v>
@@ -727,16 +747,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>10</v>
@@ -747,30 +767,36 @@
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="E10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="E11" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F11" s="4"/>
     </row>
@@ -779,12 +805,12 @@
         <v>7</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>10</v>
@@ -795,12 +821,12 @@
         <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>10</v>
@@ -808,10 +834,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -824,10 +850,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -840,10 +866,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -856,16 +882,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>18</v>
@@ -876,35 +902,37 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="E18" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F18" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>10</v>
@@ -912,19 +940,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>10</v>
@@ -932,47 +960,53 @@
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="4"/>
+        <v>58</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="E21" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="4"/>
+        <v>61</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="E22" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F22" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>10</v>
@@ -980,15 +1014,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Editados backgrounds do restaurante/estúdio foto do Castillo.
</commit_message>
<xml_diff>
--- a/Anotacoes/Mapeamento de gráficos de backgrounds.xlsx
+++ b/Anotacoes/Mapeamento de gráficos de backgrounds.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
   <si>
     <t>Versão</t>
   </si>
@@ -798,7 +798,9 @@
       <c r="E11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4" t="s">
@@ -994,7 +996,9 @@
       <c r="E22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="4"/>
+      <c r="F22" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="4" t="s">

</xml_diff>

<commit_message>
Editados backgrounds do topo da ANSA, trocando NTP por ARP.
</commit_message>
<xml_diff>
--- a/Anotacoes/Mapeamento de gráficos de backgrounds.xlsx
+++ b/Anotacoes/Mapeamento de gráficos de backgrounds.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="69">
   <si>
     <t>Versão</t>
   </si>
@@ -145,6 +145,15 @@
     <t>Recepção da ANSA (Information)</t>
   </si>
   <si>
+    <t>0x0284E4</t>
+  </si>
+  <si>
+    <t>0x0284EC</t>
+  </si>
+  <si>
+    <t>Topo da ANSA (NTP)</t>
+  </si>
+  <si>
     <t>Blue Moon</t>
   </si>
   <si>
@@ -209,6 +218,9 @@
   </si>
   <si>
     <t>0x028500</t>
+  </si>
+  <si>
+    <t>0x0284E8</t>
   </si>
 </sst>
 </file>
@@ -216,7 +228,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +249,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -246,7 +264,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -269,11 +287,18 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -285,6 +310,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -592,18 +620,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="9.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="41.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="9.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="41.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -818,7 +846,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -834,33 +862,35 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="4" t="s">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="4" t="s">
+      <c r="D14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>10</v>
@@ -868,15 +898,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>10</v>
@@ -884,45 +914,43 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>51</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>52</v>
@@ -934,27 +962,25 @@
         <v>54</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>10</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F19" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>10</v>
@@ -962,19 +988,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>10</v>
@@ -982,7 +1008,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>60</v>
@@ -994,7 +1020,7 @@
         <v>62</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>10</v>
@@ -1002,15 +1028,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="E23" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>10</v>
@@ -1018,17 +1048,51 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="A25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F25" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+      <c r="A26" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>